<commit_message>
update schedule and EC
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbgurbisz/Documents/SMR-monitoring/MRNE395-2024FA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C94A5EB-1A7B-9B40-9F1A-C67675BDFEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEB123A-0538-DD48-90AF-9A432F94439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{4525DE01-5AFE-3449-9459-0416C5161635}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{4525DE01-5AFE-3449-9459-0416C5161635}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>date</t>
   </si>
@@ -107,9 +107,6 @@
     <t>F 11/29</t>
   </si>
   <si>
-    <t>HW6</t>
-  </si>
-  <si>
     <t>HW7</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>HW5: [Monitoring station site check](https://docs.google.com/spreadsheets/d/1J3YEvWHqeVdu75PupAPLOFJHA1BwFn_1tIiBC8eVfvY/edit?gid=0#gid=0)</t>
+  </si>
+  <si>
+    <t>HW6: tie a clove hitch and cleat hitch</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,10 +1068,10 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1093,10 +1093,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1104,13 +1104,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1121,10 +1121,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1135,13 +1135,13 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1152,13 +1152,13 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1172,7 +1172,10 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1186,7 +1189,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1200,7 +1203,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1214,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1228,7 +1231,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1269,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1280,7 +1283,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
update syllabus & schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbgurbisz/Documents/SMR-monitoring/MRNE395-2025SP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbgurbisz/Documents/SMR-monitoring/MRNE395-2025FA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397C96AC-2CD0-654D-A0B4-F3A01ABF4599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D8F2A2-8923-324C-AB74-B271B9D2C1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4525DE01-5AFE-3449-9459-0416C5161635}"/>
+    <workbookView xWindow="33600" yWindow="2120" windowWidth="28800" windowHeight="17500" xr2:uid="{4525DE01-5AFE-3449-9459-0416C5161635}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>date</t>
   </si>
@@ -59,75 +59,9 @@
     <t>bring your line to class</t>
   </si>
   <si>
-    <t>Th 1/16</t>
-  </si>
-  <si>
-    <t>Th 1/23</t>
-  </si>
-  <si>
-    <t>Th 1/30</t>
-  </si>
-  <si>
-    <t>Th 2/6</t>
-  </si>
-  <si>
-    <t>Th 2/13</t>
-  </si>
-  <si>
-    <t>Th 2/20</t>
-  </si>
-  <si>
-    <t>Th 2/27</t>
-  </si>
-  <si>
-    <t>Th 3/6</t>
-  </si>
-  <si>
-    <t>Th 3/13</t>
-  </si>
-  <si>
-    <t>No class - spring break</t>
-  </si>
-  <si>
-    <t>Th 3/20</t>
-  </si>
-  <si>
-    <t>Th 3/27</t>
-  </si>
-  <si>
-    <t>Th 4/3</t>
-  </si>
-  <si>
-    <t>Th 4/10</t>
-  </si>
-  <si>
-    <t>Th 4/17</t>
-  </si>
-  <si>
-    <t>Th 4/24</t>
-  </si>
-  <si>
-    <t>[Water quality criteria](https://smr-monitoring.github.io/lesson-plans/02-wq-criteria.html)</t>
-  </si>
-  <si>
-    <t>HW1 in GC</t>
-  </si>
-  <si>
-    <t>HW2 in GC</t>
-  </si>
-  <si>
     <t>[Calibration](https://smr-monitoring.github.io/lesson-plans/03-calibration.html)</t>
   </si>
   <si>
-    <t>HW3: tie a bowline, lobster buoy hitch, and half hitch</t>
-  </si>
-  <si>
-    <t>[YSI setup](https://smr-monitoring.github.io/lesson-plans/04-ysi-setup.html)</t>
-  </si>
-  <si>
-    <t>HW4: tie a clove hitch, bowline, lobster buoy hitch, and half hitch</t>
-  </si>
-  <si>
     <t>[Continuous monitoring - practice deployment](https://smr-monitoring.github.io/lesson-plans/05-conmon.html)</t>
   </si>
   <si>
@@ -146,16 +80,106 @@
     <t>[Discrete monitoring](https://smr-monitoring.github.io/lesson-plans/09-discrete-monitoring.html)</t>
   </si>
   <si>
-    <t>HW5: tie a cleat hitch and clove hitch</t>
-  </si>
-  <si>
-    <t>[Discrete monitoring by boat](https://smr-monitoring.github.io/lesson-plans/10-discrete-boat.html)</t>
-  </si>
-  <si>
     <t>[Skills review](https://smr-monitoring.github.io/lesson-plans/11-skills-review.html)</t>
   </si>
   <si>
     <t>[Skills assessment](https://smr-monitoring.github.io/lesson-plans/12-skills-assessment.html)</t>
+  </si>
+  <si>
+    <t>F 09/05</t>
+  </si>
+  <si>
+    <t>F 09/12</t>
+  </si>
+  <si>
+    <t>F 09/19</t>
+  </si>
+  <si>
+    <t>F 09/26</t>
+  </si>
+  <si>
+    <t>F 10/10</t>
+  </si>
+  <si>
+    <t>F 10/17</t>
+  </si>
+  <si>
+    <t>F 10/24</t>
+  </si>
+  <si>
+    <t>F 10/31</t>
+  </si>
+  <si>
+    <t>F 11/07</t>
+  </si>
+  <si>
+    <t>F 11/14</t>
+  </si>
+  <si>
+    <t>F 11/21</t>
+  </si>
+  <si>
+    <t>F 11/28</t>
+  </si>
+  <si>
+    <t>F 12/05</t>
+  </si>
+  <si>
+    <t>F 12/12</t>
+  </si>
+  <si>
+    <t>[Water quality criteria and SAV](https://smr-monitoring.github.io/lesson-plans/02-wq-criteria.html)</t>
+  </si>
+  <si>
+    <t>SAV monitoring - St. Inigoes (be prepared to wade in the water)</t>
+  </si>
+  <si>
+    <t>[Discrete monitoring](https://smr-monitoring.github.io/lesson-plans/10-discrete-boat.html)</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>HW 1</t>
+  </si>
+  <si>
+    <t>HW 2</t>
+  </si>
+  <si>
+    <t>HW 3</t>
+  </si>
+  <si>
+    <t>HW 4</t>
+  </si>
+  <si>
+    <t>HW 5</t>
+  </si>
+  <si>
+    <t>HW 6</t>
+  </si>
+  <si>
+    <t>HW 7</t>
+  </si>
+  <si>
+    <t>HW 8</t>
+  </si>
+  <si>
+    <t>HW 9</t>
+  </si>
+  <si>
+    <t>HW 10</t>
+  </si>
+  <si>
+    <t>W 12/17</t>
+  </si>
+  <si>
+    <t>2:00-4:15 Final written exam</t>
+  </si>
+  <si>
+    <t>F 10/03</t>
+  </si>
+  <si>
+    <t>No class - Thanksgiving break</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1052,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,10 +1085,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1072,13 +1099,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1086,13 +1113,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1100,13 +1127,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1117,13 +1144,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1134,10 +1161,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1145,13 +1175,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1159,13 +1192,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1173,10 +1209,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1184,13 +1223,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1198,13 +1240,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1212,7 +1254,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1220,13 +1265,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1234,13 +1276,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1248,14 +1290,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>